<commit_message>
Testing stuff with different product category combinations
</commit_message>
<xml_diff>
--- a/Data/CBi_NOR.xlsx
+++ b/Data/CBi_NOR.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27612"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\GVX0EPF00012A7E\EXCELCNV\fdec2440-f3a2-487b-86d6-550f0467e7c8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{A50818C0-A461-4185-8D2D-548DEE001050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C9D042B-E091-4944-BF6A-6986B332A902}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{A50818C0-A461-4185-8D2D-548DEE001050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36D3E940-4559-4E43-9D78-E856A203AB59}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{B7DD28EE-D135-4323-B577-5415CE9104E2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="94">
   <si>
     <t>sector</t>
   </si>
@@ -1158,10 +1158,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064FCC43-3CB7-41F0-B551-E95D0B47F8E8}">
-  <dimension ref="A1:B93"/>
+  <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="B86" sqref="B85:D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1169,747 +1169,1026 @@
     <col min="1" max="1" width="116.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>47.189413612061202</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="D2">
+        <v>47.189413612031601</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <v>58.7380833602476</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="D3">
+        <v>58.738083360244502</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
         <v>44.2816946805914</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="D4">
+        <v>44.281694680581701</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
         <v>112.04612442433</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="D5">
+        <v>112.046124424308</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
         <v>39.333205569690101</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="D6">
+        <v>39.333205569688097</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7">
         <v>94.415952422167706</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="D7">
+        <v>94.415952422157901</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8">
         <v>81.086045722684304</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="D8">
+        <v>81.0860457226687</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
         <v>53.282041561425302</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="D9">
+        <v>53.282041561418701</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10">
         <v>135.68908554840201</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="D10">
+        <v>135.68908554839101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11">
         <v>51.479927151919</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="D11">
+        <v>51.479927151914403</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12">
         <v>53.395830584010703</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="D12">
+        <v>53.395830584004301</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13">
         <v>50.748768676115901</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="D13">
+        <v>50.748768676098699</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14">
         <v>386.65901138687099</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="D14">
+        <v>386.65901138684598</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15">
         <v>164.35466276120201</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="D15">
+        <v>164.354662761198</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16">
         <v>312.68760221935798</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="D16">
+        <v>312.687602219349</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17">
         <v>95.374326539322198</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="D17">
+        <v>95.374326539297201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18">
         <v>41.067977955722398</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="D18">
+        <v>41.067977955707804</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19">
         <v>102.64437028589001</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="D19">
+        <v>102.64437028577299</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20">
         <v>45.926158487475902</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="D20">
+        <v>45.926158487472101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21">
         <v>46.5641180203896</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="D21">
+        <v>46.564118020385102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22">
         <v>35.137031853302503</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="D22">
+        <v>35.137031853292001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23">
         <v>43.983733953717298</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="D23">
+        <v>43.983733953707201</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24">
         <v>218.52180976470501</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="D24">
+        <v>218.52180976469799</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25">
         <v>138.20530932191801</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="D25">
+        <v>138.20530932192099</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26">
         <v>28.667477598784401</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="D26">
+        <v>28.6674775987745</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27">
         <v>106.234941636214</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="D27">
+        <v>106.234941636199</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>28</v>
       </c>
       <c r="B28">
         <v>368.74045422218899</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="D28">
+        <v>368.74045422218597</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>29</v>
       </c>
       <c r="B29">
         <v>64.518981971621201</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="D29">
+        <v>64.518981971608795</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30">
         <v>797.75015076416696</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="D30">
+        <v>797.75015076397005</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31">
         <v>100.87766898682</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="D31">
+        <v>100.877668986823</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>32</v>
       </c>
       <c r="B32">
         <v>109.42149670223699</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="D32">
+        <v>109.421496702224</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>33</v>
       </c>
       <c r="B33">
         <v>144.33575947775699</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="D33">
+        <v>144.33575947774699</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>34</v>
       </c>
       <c r="B34">
         <v>48.874210485501898</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="D34">
+        <v>48.874210485486898</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35">
         <v>143.78196519994199</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="D35">
+        <v>143.78196519989399</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>36</v>
       </c>
       <c r="B36">
         <v>51.388989757544302</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="D36">
+        <v>51.388989757533402</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>37</v>
       </c>
       <c r="B37">
         <v>86.706898898612295</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="D37">
+        <v>86.706898898595</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>38</v>
       </c>
       <c r="B38">
         <v>89.341393943738694</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
+      <c r="D38">
+        <v>89.341393943718501</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>39</v>
       </c>
       <c r="B39">
         <v>102.404210676012</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="D39">
+        <v>102.404210675996</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>40</v>
       </c>
       <c r="B40">
         <v>116.937246126555</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="D40">
+        <v>116.937246126544</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>41</v>
       </c>
       <c r="B41">
         <v>39.764176175346599</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="D41">
+        <v>39.764176175339998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>42</v>
       </c>
       <c r="B42">
         <v>182.625351657213</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
+      <c r="D42">
+        <v>182.625351657198</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>43</v>
       </c>
       <c r="B43">
         <v>102.918489137029</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="D43">
+        <v>102.91848913702</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>44</v>
       </c>
       <c r="B44">
         <v>104.668229073535</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="D44">
+        <v>104.668229073487</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>45</v>
       </c>
       <c r="B45">
         <v>52.148399168253803</v>
       </c>
-    </row>
-    <row r="46" spans="1:2">
+      <c r="D45">
+        <v>52.148399168236402</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
         <v>46</v>
       </c>
       <c r="B46">
         <v>131.16814949540799</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
+      <c r="D46">
+        <v>131.16814949537701</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>47</v>
       </c>
       <c r="B47">
         <v>228.71282360238499</v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
+      <c r="D47">
+        <v>228.712823602306</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>48</v>
       </c>
       <c r="B48">
         <v>89.568262540323204</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
+      <c r="D48">
+        <v>89.568262540305994</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>49</v>
       </c>
       <c r="B49">
         <v>134.72921425628101</v>
       </c>
-    </row>
-    <row r="50" spans="1:2">
+      <c r="D49">
+        <v>134.729214256266</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>50</v>
       </c>
       <c r="B50">
         <v>160.953494218923</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
+      <c r="D50">
+        <v>160.95349421880101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>51</v>
       </c>
       <c r="B51">
         <v>89.840918428095407</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="D51">
+        <v>89.840918428082603</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>52</v>
       </c>
       <c r="B52">
         <v>127.446315271598</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
+      <c r="D52">
+        <v>127.446315271572</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
         <v>53</v>
       </c>
       <c r="B53">
         <v>279.60754606800202</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
+      <c r="D53">
+        <v>279.60754606795598</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
         <v>54</v>
       </c>
       <c r="B54">
         <v>457.2373660257</v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
+      <c r="D54">
+        <v>457.23736602569699</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
         <v>55</v>
       </c>
       <c r="B55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
+      <c r="D55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>56</v>
       </c>
       <c r="B56">
         <v>367.44215918850603</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
+      <c r="D56">
+        <v>367.44215918850301</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
         <v>57</v>
       </c>
       <c r="B57">
         <v>1195.73850723961</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
+      <c r="D57">
+        <v>1195.7385072396</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
         <v>58</v>
       </c>
       <c r="B58">
         <v>11.060972679280299</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
+      <c r="D58">
+        <v>11.060972679280701</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
         <v>59</v>
       </c>
       <c r="B59">
         <v>601.69460500271703</v>
       </c>
-    </row>
-    <row r="60" spans="1:2">
+      <c r="D59">
+        <v>601.69460500270702</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
         <v>60</v>
       </c>
       <c r="B60">
         <v>439.54417329656701</v>
       </c>
-    </row>
-    <row r="61" spans="1:2">
+      <c r="D60">
+        <v>439.54417329655399</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" t="s">
         <v>61</v>
       </c>
       <c r="B61">
         <v>883.80411528028299</v>
       </c>
-    </row>
-    <row r="62" spans="1:2">
+      <c r="D61">
+        <v>883.80411528027605</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62" t="s">
         <v>62</v>
       </c>
       <c r="B62">
         <v>57.2141021741825</v>
       </c>
-    </row>
-    <row r="63" spans="1:2">
+      <c r="D62">
+        <v>57.214102174169398</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63" t="s">
         <v>63</v>
       </c>
       <c r="B63">
         <v>279.77315035840201</v>
       </c>
-    </row>
-    <row r="64" spans="1:2">
+      <c r="D63">
+        <v>279.77315035835198</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64" t="s">
         <v>64</v>
       </c>
       <c r="B64">
         <v>36.0154730329903</v>
       </c>
-    </row>
-    <row r="65" spans="1:2">
+      <c r="D64">
+        <v>36.015473032969197</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65" t="s">
         <v>65</v>
       </c>
       <c r="B65">
         <v>12.345559320836299</v>
       </c>
-    </row>
-    <row r="66" spans="1:2">
+      <c r="D65">
+        <v>12.3455593208305</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66" t="s">
         <v>66</v>
       </c>
       <c r="B66">
         <v>15.1126225541369</v>
       </c>
-    </row>
-    <row r="67" spans="1:2">
+      <c r="D66">
+        <v>15.1126225541346</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
         <v>67</v>
       </c>
       <c r="B67">
         <v>19.988445783937198</v>
       </c>
-    </row>
-    <row r="68" spans="1:2">
+      <c r="D67">
+        <v>19.988445783934601</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" t="s">
         <v>68</v>
       </c>
       <c r="B68">
         <v>39.269256088968298</v>
       </c>
-    </row>
-    <row r="69" spans="1:2">
+      <c r="D68">
+        <v>39.269256088968397</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69" t="s">
         <v>69</v>
       </c>
       <c r="B69">
         <v>46.366184165183199</v>
       </c>
-    </row>
-    <row r="70" spans="1:2">
+      <c r="D69">
+        <v>46.366184165177103</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70" t="s">
         <v>70</v>
       </c>
       <c r="B70">
         <v>44.311439128336303</v>
       </c>
-    </row>
-    <row r="71" spans="1:2">
+      <c r="D70">
+        <v>44.3114391283356</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71" t="s">
         <v>71</v>
       </c>
       <c r="B71">
         <v>150.368250150991</v>
       </c>
-    </row>
-    <row r="72" spans="1:2">
+      <c r="D71">
+        <v>150.368250150981</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72" t="s">
         <v>72</v>
       </c>
       <c r="B72">
         <v>28327.550188678601</v>
       </c>
-    </row>
-    <row r="73" spans="1:2">
+      <c r="D72">
+        <v>28327.550188678499</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73" t="s">
         <v>73</v>
       </c>
       <c r="B73">
         <v>110.370512301872</v>
       </c>
-    </row>
-    <row r="74" spans="1:2">
+      <c r="D73">
+        <v>110.370512301864</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74" t="s">
         <v>74</v>
       </c>
       <c r="B74">
         <v>41.2872142595497</v>
       </c>
-    </row>
-    <row r="75" spans="1:2">
+      <c r="D74">
+        <v>41.2872142595266</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75" t="s">
         <v>75</v>
       </c>
       <c r="B75">
         <v>20.406128906077001</v>
       </c>
-    </row>
-    <row r="76" spans="1:2">
+      <c r="D75">
+        <v>20.406128906071501</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76" t="s">
         <v>76</v>
       </c>
       <c r="B76">
         <v>13.186696677533901</v>
       </c>
-    </row>
-    <row r="77" spans="1:2">
+      <c r="D76">
+        <v>13.186696677522001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77" t="s">
         <v>77</v>
       </c>
       <c r="B77">
         <v>19.632107103967499</v>
       </c>
-    </row>
-    <row r="78" spans="1:2">
+      <c r="D77">
+        <v>19.6321071039605</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78" t="s">
         <v>78</v>
       </c>
       <c r="B78">
         <v>46.826601475078597</v>
       </c>
-    </row>
-    <row r="79" spans="1:2">
+      <c r="D78">
+        <v>46.826601475067498</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
       <c r="A79" t="s">
         <v>79</v>
       </c>
       <c r="B79">
         <v>70.411624441820507</v>
       </c>
-    </row>
-    <row r="80" spans="1:2">
+      <c r="D79">
+        <v>70.411624441789598</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" t="s">
         <v>80</v>
       </c>
       <c r="B80">
         <v>117.480877676307</v>
       </c>
-    </row>
-    <row r="81" spans="1:2">
+      <c r="D80">
+        <v>117.48087767625201</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
       <c r="A81" t="s">
         <v>81</v>
       </c>
       <c r="B81">
         <v>31.160322645513599</v>
       </c>
-    </row>
-    <row r="82" spans="1:2">
+      <c r="D81">
+        <v>31.160322645503701</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
       <c r="A82" t="s">
         <v>82</v>
       </c>
       <c r="B82">
         <v>277.86045513357698</v>
       </c>
-    </row>
-    <row r="83" spans="1:2">
+      <c r="D82">
+        <v>277.86045513357698</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
       <c r="A83" t="s">
         <v>83</v>
       </c>
       <c r="B83">
         <v>133.28489008696499</v>
       </c>
-    </row>
-    <row r="84" spans="1:2">
+      <c r="D83">
+        <v>133.28489008693299</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
       <c r="A84" t="s">
         <v>84</v>
       </c>
       <c r="B84">
         <v>105.841415679102</v>
       </c>
-    </row>
-    <row r="85" spans="1:2">
+      <c r="D84">
+        <v>105.841415679091</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
       <c r="A85" t="s">
         <v>85</v>
       </c>
       <c r="B85">
         <v>77.075657857210999</v>
       </c>
-    </row>
-    <row r="86" spans="1:2">
+      <c r="D85">
+        <v>77.0756578571971</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
       <c r="A86" t="s">
         <v>86</v>
       </c>
       <c r="B86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:2">
+      <c r="D86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
       <c r="A87" t="s">
         <v>87</v>
       </c>
       <c r="B87">
         <v>69.210845057274099</v>
       </c>
-    </row>
-    <row r="88" spans="1:2">
+      <c r="D87">
+        <v>69.210845057260101</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
       <c r="A88" t="s">
         <v>88</v>
       </c>
       <c r="B88">
         <v>64.252323390701804</v>
       </c>
-    </row>
-    <row r="89" spans="1:2">
+      <c r="D88">
+        <v>64.252323390676906</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
       <c r="A89" t="s">
         <v>89</v>
       </c>
       <c r="B89">
         <v>624.05146076451399</v>
       </c>
-    </row>
-    <row r="90" spans="1:2">
+      <c r="D89">
+        <v>624.05146076423205</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
       <c r="A90" t="s">
         <v>90</v>
       </c>
       <c r="B90">
         <v>173.107188453276</v>
       </c>
-    </row>
-    <row r="91" spans="1:2">
+      <c r="D90">
+        <v>173.10718845322401</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
       <c r="A91" t="s">
         <v>91</v>
       </c>
       <c r="B91">
         <v>23.869309194376999</v>
       </c>
-    </row>
-    <row r="92" spans="1:2">
+      <c r="D91">
+        <v>23.869309194377301</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
       <c r="A92" t="s">
         <v>92</v>
       </c>
       <c r="B92">
         <v>3.2020811100273101</v>
       </c>
-    </row>
-    <row r="93" spans="1:2">
+      <c r="D92">
+        <v>3.2020811100272701</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
       <c r="A93" t="s">
         <v>93</v>
       </c>
       <c r="B93">
+        <v>0</v>
+      </c>
+      <c r="D93">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Plotting even more stuff
</commit_message>
<xml_diff>
--- a/Data/CBi_NOR.xlsx
+++ b/Data/CBi_NOR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\GVX0EPF00012A7E\EXCELCNV\fdec2440-f3a2-487b-86d6-550f0467e7c8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{A50818C0-A461-4185-8D2D-548DEE001050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36D3E940-4559-4E43-9D78-E856A203AB59}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{A50818C0-A461-4185-8D2D-548DEE001050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{502AD95E-FF06-4A35-A4A1-F3805914CA82}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{B7DD28EE-D135-4323-B577-5415CE9104E2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>sector</t>
   </si>
@@ -1158,10 +1158,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064FCC43-3CB7-41F0-B551-E95D0B47F8E8}">
-  <dimension ref="A1:D93"/>
+  <dimension ref="A1:B93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="B86" sqref="B85:D86"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1169,1026 +1169,747 @@
     <col min="1" max="1" width="116.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>47.189413612061202</v>
       </c>
-      <c r="D2">
-        <v>47.189413612031601</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <v>58.7380833602476</v>
       </c>
-      <c r="D3">
-        <v>58.738083360244502</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
         <v>44.2816946805914</v>
       </c>
-      <c r="D4">
-        <v>44.281694680581701</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
         <v>112.04612442433</v>
       </c>
-      <c r="D5">
-        <v>112.046124424308</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
         <v>39.333205569690101</v>
       </c>
-      <c r="D6">
-        <v>39.333205569688097</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7">
         <v>94.415952422167706</v>
       </c>
-      <c r="D7">
-        <v>94.415952422157901</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8">
         <v>81.086045722684304</v>
       </c>
-      <c r="D8">
-        <v>81.0860457226687</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
         <v>53.282041561425302</v>
       </c>
-      <c r="D9">
-        <v>53.282041561418701</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10">
         <v>135.68908554840201</v>
       </c>
-      <c r="D10">
-        <v>135.68908554839101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11">
         <v>51.479927151919</v>
       </c>
-      <c r="D11">
-        <v>51.479927151914403</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12">
         <v>53.395830584010703</v>
       </c>
-      <c r="D12">
-        <v>53.395830584004301</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13">
         <v>50.748768676115901</v>
       </c>
-      <c r="D13">
-        <v>50.748768676098699</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14">
         <v>386.65901138687099</v>
       </c>
-      <c r="D14">
-        <v>386.65901138684598</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15">
         <v>164.35466276120201</v>
       </c>
-      <c r="D15">
-        <v>164.354662761198</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16">
         <v>312.68760221935798</v>
       </c>
-      <c r="D16">
-        <v>312.687602219349</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17">
         <v>95.374326539322198</v>
       </c>
-      <c r="D17">
-        <v>95.374326539297201</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18">
         <v>41.067977955722398</v>
       </c>
-      <c r="D18">
-        <v>41.067977955707804</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19">
         <v>102.64437028589001</v>
       </c>
-      <c r="D19">
-        <v>102.64437028577299</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20">
         <v>45.926158487475902</v>
       </c>
-      <c r="D20">
-        <v>45.926158487472101</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21">
         <v>46.5641180203896</v>
       </c>
-      <c r="D21">
-        <v>46.564118020385102</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22">
         <v>35.137031853302503</v>
       </c>
-      <c r="D22">
-        <v>35.137031853292001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23">
         <v>43.983733953717298</v>
       </c>
-      <c r="D23">
-        <v>43.983733953707201</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24">
         <v>218.52180976470501</v>
       </c>
-      <c r="D24">
-        <v>218.52180976469799</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25">
         <v>138.20530932191801</v>
       </c>
-      <c r="D25">
-        <v>138.20530932192099</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26">
         <v>28.667477598784401</v>
       </c>
-      <c r="D26">
-        <v>28.6674775987745</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27">
         <v>106.234941636214</v>
       </c>
-      <c r="D27">
-        <v>106.234941636199</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
       <c r="B28">
         <v>368.74045422218899</v>
       </c>
-      <c r="D28">
-        <v>368.74045422218597</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
       <c r="B29">
         <v>64.518981971621201</v>
       </c>
-      <c r="D29">
-        <v>64.518981971608795</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30">
         <v>797.75015076416696</v>
       </c>
-      <c r="D30">
-        <v>797.75015076397005</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31">
         <v>100.87766898682</v>
       </c>
-      <c r="D31">
-        <v>100.877668986823</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>32</v>
       </c>
       <c r="B32">
         <v>109.42149670223699</v>
       </c>
-      <c r="D32">
-        <v>109.421496702224</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>33</v>
       </c>
       <c r="B33">
         <v>144.33575947775699</v>
       </c>
-      <c r="D33">
-        <v>144.33575947774699</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>34</v>
       </c>
       <c r="B34">
         <v>48.874210485501898</v>
       </c>
-      <c r="D34">
-        <v>48.874210485486898</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35">
         <v>143.78196519994199</v>
       </c>
-      <c r="D35">
-        <v>143.78196519989399</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>36</v>
       </c>
       <c r="B36">
         <v>51.388989757544302</v>
       </c>
-      <c r="D36">
-        <v>51.388989757533402</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>37</v>
       </c>
       <c r="B37">
         <v>86.706898898612295</v>
       </c>
-      <c r="D37">
-        <v>86.706898898595</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>38</v>
       </c>
       <c r="B38">
         <v>89.341393943738694</v>
       </c>
-      <c r="D38">
-        <v>89.341393943718501</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
+    </row>
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>39</v>
       </c>
       <c r="B39">
         <v>102.404210676012</v>
       </c>
-      <c r="D39">
-        <v>102.404210675996</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
+    </row>
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>40</v>
       </c>
       <c r="B40">
         <v>116.937246126555</v>
       </c>
-      <c r="D40">
-        <v>116.937246126544</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
+    </row>
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>41</v>
       </c>
       <c r="B41">
         <v>39.764176175346599</v>
       </c>
-      <c r="D41">
-        <v>39.764176175339998</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+    </row>
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>42</v>
       </c>
       <c r="B42">
         <v>182.625351657213</v>
       </c>
-      <c r="D42">
-        <v>182.625351657198</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
+    </row>
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>43</v>
       </c>
       <c r="B43">
         <v>102.918489137029</v>
       </c>
-      <c r="D43">
-        <v>102.91848913702</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
+    </row>
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>44</v>
       </c>
       <c r="B44">
         <v>104.668229073535</v>
       </c>
-      <c r="D44">
-        <v>104.668229073487</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
+    </row>
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>45</v>
       </c>
       <c r="B45">
         <v>52.148399168253803</v>
       </c>
-      <c r="D45">
-        <v>52.148399168236402</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
+    </row>
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>46</v>
       </c>
       <c r="B46">
         <v>131.16814949540799</v>
       </c>
-      <c r="D46">
-        <v>131.16814949537701</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
+    </row>
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>47</v>
       </c>
       <c r="B47">
         <v>228.71282360238499</v>
       </c>
-      <c r="D47">
-        <v>228.712823602306</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
+    </row>
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>48</v>
       </c>
       <c r="B48">
         <v>89.568262540323204</v>
       </c>
-      <c r="D48">
-        <v>89.568262540305994</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
+    </row>
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>49</v>
       </c>
       <c r="B49">
         <v>134.72921425628101</v>
       </c>
-      <c r="D49">
-        <v>134.729214256266</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
+    </row>
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>50</v>
       </c>
       <c r="B50">
         <v>160.953494218923</v>
       </c>
-      <c r="D50">
-        <v>160.95349421880101</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
+    </row>
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
         <v>51</v>
       </c>
       <c r="B51">
         <v>89.840918428095407</v>
       </c>
-      <c r="D51">
-        <v>89.840918428082603</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
+    </row>
+    <row r="52" spans="1:2">
       <c r="A52" t="s">
         <v>52</v>
       </c>
       <c r="B52">
         <v>127.446315271598</v>
       </c>
-      <c r="D52">
-        <v>127.446315271572</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
+    </row>
+    <row r="53" spans="1:2">
       <c r="A53" t="s">
         <v>53</v>
       </c>
       <c r="B53">
         <v>279.60754606800202</v>
       </c>
-      <c r="D53">
-        <v>279.60754606795598</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
+    </row>
+    <row r="54" spans="1:2">
       <c r="A54" t="s">
         <v>54</v>
       </c>
       <c r="B54">
         <v>457.2373660257</v>
       </c>
-      <c r="D54">
-        <v>457.23736602569699</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
+    </row>
+    <row r="55" spans="1:2">
       <c r="A55" t="s">
         <v>55</v>
       </c>
       <c r="B55">
         <v>0</v>
       </c>
-      <c r="D55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
+    </row>
+    <row r="56" spans="1:2">
       <c r="A56" t="s">
         <v>56</v>
       </c>
       <c r="B56">
         <v>367.44215918850603</v>
       </c>
-      <c r="D56">
-        <v>367.44215918850301</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
+    </row>
+    <row r="57" spans="1:2">
       <c r="A57" t="s">
         <v>57</v>
       </c>
       <c r="B57">
         <v>1195.73850723961</v>
       </c>
-      <c r="D57">
-        <v>1195.7385072396</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
+    </row>
+    <row r="58" spans="1:2">
       <c r="A58" t="s">
         <v>58</v>
       </c>
       <c r="B58">
         <v>11.060972679280299</v>
       </c>
-      <c r="D58">
-        <v>11.060972679280701</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
+    </row>
+    <row r="59" spans="1:2">
       <c r="A59" t="s">
         <v>59</v>
       </c>
       <c r="B59">
         <v>601.69460500271703</v>
       </c>
-      <c r="D59">
-        <v>601.69460500270702</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
+    </row>
+    <row r="60" spans="1:2">
       <c r="A60" t="s">
         <v>60</v>
       </c>
       <c r="B60">
         <v>439.54417329656701</v>
       </c>
-      <c r="D60">
-        <v>439.54417329655399</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
+    </row>
+    <row r="61" spans="1:2">
       <c r="A61" t="s">
         <v>61</v>
       </c>
       <c r="B61">
         <v>883.80411528028299</v>
       </c>
-      <c r="D61">
-        <v>883.80411528027605</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
+    </row>
+    <row r="62" spans="1:2">
       <c r="A62" t="s">
         <v>62</v>
       </c>
       <c r="B62">
         <v>57.2141021741825</v>
       </c>
-      <c r="D62">
-        <v>57.214102174169398</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
+    </row>
+    <row r="63" spans="1:2">
       <c r="A63" t="s">
         <v>63</v>
       </c>
       <c r="B63">
         <v>279.77315035840201</v>
       </c>
-      <c r="D63">
-        <v>279.77315035835198</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
+    </row>
+    <row r="64" spans="1:2">
       <c r="A64" t="s">
         <v>64</v>
       </c>
       <c r="B64">
         <v>36.0154730329903</v>
       </c>
-      <c r="D64">
-        <v>36.015473032969197</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
+    </row>
+    <row r="65" spans="1:2">
       <c r="A65" t="s">
         <v>65</v>
       </c>
       <c r="B65">
         <v>12.345559320836299</v>
       </c>
-      <c r="D65">
-        <v>12.3455593208305</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
+    </row>
+    <row r="66" spans="1:2">
       <c r="A66" t="s">
         <v>66</v>
       </c>
       <c r="B66">
         <v>15.1126225541369</v>
       </c>
-      <c r="D66">
-        <v>15.1126225541346</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
+    </row>
+    <row r="67" spans="1:2">
       <c r="A67" t="s">
         <v>67</v>
       </c>
       <c r="B67">
         <v>19.988445783937198</v>
       </c>
-      <c r="D67">
-        <v>19.988445783934601</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
+    </row>
+    <row r="68" spans="1:2">
       <c r="A68" t="s">
         <v>68</v>
       </c>
       <c r="B68">
         <v>39.269256088968298</v>
       </c>
-      <c r="D68">
-        <v>39.269256088968397</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
+    </row>
+    <row r="69" spans="1:2">
       <c r="A69" t="s">
         <v>69</v>
       </c>
       <c r="B69">
         <v>46.366184165183199</v>
       </c>
-      <c r="D69">
-        <v>46.366184165177103</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
+    </row>
+    <row r="70" spans="1:2">
       <c r="A70" t="s">
         <v>70</v>
       </c>
       <c r="B70">
         <v>44.311439128336303</v>
       </c>
-      <c r="D70">
-        <v>44.3114391283356</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
+    </row>
+    <row r="71" spans="1:2">
       <c r="A71" t="s">
         <v>71</v>
       </c>
       <c r="B71">
         <v>150.368250150991</v>
       </c>
-      <c r="D71">
-        <v>150.368250150981</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
+    </row>
+    <row r="72" spans="1:2">
       <c r="A72" t="s">
         <v>72</v>
       </c>
       <c r="B72">
         <v>28327.550188678601</v>
       </c>
-      <c r="D72">
-        <v>28327.550188678499</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
+    </row>
+    <row r="73" spans="1:2">
       <c r="A73" t="s">
         <v>73</v>
       </c>
       <c r="B73">
         <v>110.370512301872</v>
       </c>
-      <c r="D73">
-        <v>110.370512301864</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
+    </row>
+    <row r="74" spans="1:2">
       <c r="A74" t="s">
         <v>74</v>
       </c>
       <c r="B74">
         <v>41.2872142595497</v>
       </c>
-      <c r="D74">
-        <v>41.2872142595266</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
+    </row>
+    <row r="75" spans="1:2">
       <c r="A75" t="s">
         <v>75</v>
       </c>
       <c r="B75">
         <v>20.406128906077001</v>
       </c>
-      <c r="D75">
-        <v>20.406128906071501</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
+    </row>
+    <row r="76" spans="1:2">
       <c r="A76" t="s">
         <v>76</v>
       </c>
       <c r="B76">
         <v>13.186696677533901</v>
       </c>
-      <c r="D76">
-        <v>13.186696677522001</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
+    </row>
+    <row r="77" spans="1:2">
       <c r="A77" t="s">
         <v>77</v>
       </c>
       <c r="B77">
         <v>19.632107103967499</v>
       </c>
-      <c r="D77">
-        <v>19.6321071039605</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
+    </row>
+    <row r="78" spans="1:2">
       <c r="A78" t="s">
         <v>78</v>
       </c>
       <c r="B78">
         <v>46.826601475078597</v>
       </c>
-      <c r="D78">
-        <v>46.826601475067498</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
+    </row>
+    <row r="79" spans="1:2">
       <c r="A79" t="s">
         <v>79</v>
       </c>
       <c r="B79">
         <v>70.411624441820507</v>
       </c>
-      <c r="D79">
-        <v>70.411624441789598</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4">
+    </row>
+    <row r="80" spans="1:2">
       <c r="A80" t="s">
         <v>80</v>
       </c>
       <c r="B80">
         <v>117.480877676307</v>
       </c>
-      <c r="D80">
-        <v>117.48087767625201</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4">
+    </row>
+    <row r="81" spans="1:2">
       <c r="A81" t="s">
         <v>81</v>
       </c>
       <c r="B81">
         <v>31.160322645513599</v>
       </c>
-      <c r="D81">
-        <v>31.160322645503701</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
+    </row>
+    <row r="82" spans="1:2">
       <c r="A82" t="s">
         <v>82</v>
       </c>
       <c r="B82">
         <v>277.86045513357698</v>
       </c>
-      <c r="D82">
-        <v>277.86045513357698</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4">
+    </row>
+    <row r="83" spans="1:2">
       <c r="A83" t="s">
         <v>83</v>
       </c>
       <c r="B83">
         <v>133.28489008696499</v>
       </c>
-      <c r="D83">
-        <v>133.28489008693299</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4">
+    </row>
+    <row r="84" spans="1:2">
       <c r="A84" t="s">
         <v>84</v>
       </c>
       <c r="B84">
         <v>105.841415679102</v>
       </c>
-      <c r="D84">
-        <v>105.841415679091</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4">
+    </row>
+    <row r="85" spans="1:2">
       <c r="A85" t="s">
         <v>85</v>
       </c>
       <c r="B85">
         <v>77.075657857210999</v>
       </c>
-      <c r="D85">
-        <v>77.0756578571971</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4">
+    </row>
+    <row r="86" spans="1:2">
       <c r="A86" t="s">
         <v>86</v>
       </c>
       <c r="B86">
         <v>0</v>
       </c>
-      <c r="D86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4">
+    </row>
+    <row r="87" spans="1:2">
       <c r="A87" t="s">
         <v>87</v>
       </c>
       <c r="B87">
         <v>69.210845057274099</v>
       </c>
-      <c r="D87">
-        <v>69.210845057260101</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4">
+    </row>
+    <row r="88" spans="1:2">
       <c r="A88" t="s">
         <v>88</v>
       </c>
       <c r="B88">
         <v>64.252323390701804</v>
       </c>
-      <c r="D88">
-        <v>64.252323390676906</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4">
+    </row>
+    <row r="89" spans="1:2">
       <c r="A89" t="s">
         <v>89</v>
       </c>
       <c r="B89">
         <v>624.05146076451399</v>
       </c>
-      <c r="D89">
-        <v>624.05146076423205</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4">
+    </row>
+    <row r="90" spans="1:2">
       <c r="A90" t="s">
         <v>90</v>
       </c>
       <c r="B90">
         <v>173.107188453276</v>
       </c>
-      <c r="D90">
-        <v>173.10718845322401</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4">
+    </row>
+    <row r="91" spans="1:2">
       <c r="A91" t="s">
         <v>91</v>
       </c>
       <c r="B91">
         <v>23.869309194376999</v>
       </c>
-      <c r="D91">
-        <v>23.869309194377301</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4">
+    </row>
+    <row r="92" spans="1:2">
       <c r="A92" t="s">
         <v>92</v>
       </c>
       <c r="B92">
         <v>3.2020811100273101</v>
       </c>
-      <c r="D92">
-        <v>3.2020811100272701</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4">
+    </row>
+    <row r="93" spans="1:2">
       <c r="A93" t="s">
         <v>93</v>
       </c>
       <c r="B93">
-        <v>0</v>
-      </c>
-      <c r="D93">
         <v>0</v>
       </c>
     </row>

</xml_diff>